<commit_message>
Combined weakness in dataframe and exported to excel
</commit_message>
<xml_diff>
--- a/Code/Dataframe reference.xlsx
+++ b/Code/Dataframe reference.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepak/RWTH Academic/Fourth semester/Thesis/padsThesis/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B814E82-C596-B041-92B3-CC820685760F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E8725D-D3BD-654A-A142-D14A6ECDF39D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14020" xr2:uid="{0D4C039F-695B-A14E-A2A9-200302069A89}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>Detected Weakness Row</t>
   </si>
@@ -631,7 +631,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -937,8 +937,8 @@
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2</v>
+      <c r="A14" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Performance aspect case and activity duration
</commit_message>
<xml_diff>
--- a/Code/Dataframe reference.xlsx
+++ b/Code/Dataframe reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepak/RWTH Academic/Fourth semester/Thesis/padsThesis/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E8725D-D3BD-654A-A142-D14A6ECDF39D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA17EA2-7755-4F46-B2DF-A0D6EA78FEFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14020" xr2:uid="{0D4C039F-695B-A14E-A2A9-200302069A89}"/>
+    <workbookView xWindow="480" yWindow="920" windowWidth="25040" windowHeight="14020" xr2:uid="{0D4C039F-695B-A14E-A2A9-200302069A89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Detected Weakness Row</t>
   </si>
@@ -58,24 +58,6 @@
     <t>Weakness Measurement</t>
   </si>
   <si>
-    <t xml:space="preserve">110/02/2020 12:20 </t>
-  </si>
-  <si>
-    <t>Case 18</t>
-  </si>
-  <si>
-    <t>Pa</t>
-  </si>
-  <si>
-    <t>Auto</t>
-  </si>
-  <si>
-    <t>Long duration of the case</t>
-  </si>
-  <si>
-    <t>20% longer than average case duration</t>
-  </si>
-  <si>
     <t>Weakness type</t>
   </si>
   <si>
@@ -206,13 +188,46 @@
   </si>
   <si>
     <t>Parallelizable tasks :[('Turning &amp; Milling - Machine 9', 'Turning &amp; Milling - Machine 6'), ('Turning &amp; Milling Q.C.', 'Turning &amp; Milling - Machine 9')]</t>
+  </si>
+  <si>
+    <t>Cases and |duration - mean duration|</t>
+  </si>
+  <si>
+    <t>Case 178-&gt; Event 0</t>
+  </si>
+  <si>
+    <t>Case 178</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Distance from average activity duration</t>
+  </si>
+  <si>
+    <t>Activity level</t>
+  </si>
+  <si>
+    <t>Case 99</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Distance from median case duration in seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,18 +242,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,14 +261,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1E1E1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -279,41 +283,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13141EF3-9AE3-1F45-AA00-102E70E39C57}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,320 +632,358 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="4">
+        <v>41183</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4">
+        <v>41183.604166666664</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="6">
-        <v>41183</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3">
+        <v>7</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="5">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="6">
-        <v>41183.604166666664</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="5">
-        <v>7</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
+      <c r="G14" s="3">
+        <v>549420</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5">
-        <v>8</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5">
-        <v>9</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5">
+        <v>40910</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3600</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3">
-        <v>5</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="5"/>
+      <c r="I15" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -970,10 +992,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3418E9E3-DBF2-CD40-8885-309F39E525B4}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,112 +1005,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>